<commit_message>
reverse code in manual
</commit_message>
<xml_diff>
--- a/data_analysis/manuale_questionario.xlsx
+++ b/data_analysis/manuale_questionario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rocpa\OneDrive\Documenti\GitHub\GENOVA_wya\archiviati\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rocpa\OneDrive\Documenti\GitHub\tragedynatural\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0DA7F2-2389-4D34-94E4-3A0A4A9B3004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25822A92-0970-4CE3-B6B6-93F1D9DD43ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2ADF30A5-3C9B-44A1-8FFC-5B23687E1561}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2ADF30A5-3C9B-44A1-8FFC-5B23687E1561}"/>
   </bookViews>
   <sheets>
     <sheet name="studenti24_genova" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="130">
   <si>
     <t>StartDate</t>
   </si>
@@ -439,6 +439,9 @@
   </si>
   <si>
     <t>Sessione (LUOGO 2 digit, PROGRESSIVO 2 digit, e.g. GE02; GE00 unknown)</t>
+  </si>
+  <si>
+    <t>Variabili da ricodificare recode</t>
   </si>
 </sst>
 </file>
@@ -810,13 +813,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{425DCCE1-ED76-4D8C-8646-701A174793C3}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="M58" sqref="M58"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.5546875" customWidth="1"/>
+    <col min="2" max="2" width="152" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1232,6 +1239,31 @@
       </c>
       <c r="B52" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>